<commit_message>
add the transformation to annual report logs
</commit_message>
<xml_diff>
--- a/mapping_spreadsheet/Casrec_Mapping_Document_Reporting.xlsx
+++ b/mapping_spreadsheet/Casrec_Mapping_Document_Reporting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifermackown/Documents/work/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41EF53C8-5695-2C4C-85AB-3B994A19807D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{804E9ED9-24E9-FE4F-887D-EDBBA764A3BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17200" yWindow="460" windowWidth="34400" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="107">
   <si>
     <t>table_name</t>
   </si>
@@ -347,6 +347,9 @@
   </si>
   <si>
     <t>get_max_col</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -692,9 +695,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K13" sqref="K13"/>
+      <selection pane="bottomLeft" activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -703,11 +706,11 @@
     <col min="2" max="2" width="9.1640625" customWidth="1"/>
     <col min="3" max="3" width="26.1640625" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
-    <col min="5" max="5" width="6" customWidth="1"/>
-    <col min="6" max="6" width="119.5" customWidth="1"/>
-    <col min="7" max="7" width="12.83203125" customWidth="1"/>
+    <col min="5" max="5" width="6" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="119.5" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="9" max="9" width="19.83203125" customWidth="1"/>
+    <col min="9" max="9" width="19.83203125" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="20" customWidth="1"/>
     <col min="11" max="11" width="22.5" customWidth="1"/>
     <col min="12" max="12" width="12.5" customWidth="1"/>
@@ -1025,6 +1028,9 @@
       </c>
       <c r="K12" t="s">
         <v>105</v>
+      </c>
+      <c r="P12" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
some dates are required but we don't have a calc yet so defaulting to current_date
missing another default field
</commit_message>
<xml_diff>
--- a/mapping_spreadsheet/Casrec_Mapping_Document_Reporting.xlsx
+++ b/mapping_spreadsheet/Casrec_Mapping_Document_Reporting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifermackown/Documents/work/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{804E9ED9-24E9-FE4F-887D-EDBBA764A3BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EC3996F-5837-C149-8A0B-C30877783F04}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17200" yWindow="460" windowWidth="34400" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45880" yWindow="460" windowWidth="22920" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="annual_report_logs" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="108">
   <si>
     <t>table_name</t>
   </si>
@@ -351,12 +351,15 @@
   <si>
     <t>yes</t>
   </si>
+  <si>
+    <t>current_date</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -393,6 +396,12 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -442,7 +451,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -478,6 +487,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -695,9 +709,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P12" sqref="P12"/>
+      <selection pane="bottomLeft" activeCell="M1" sqref="M1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -714,7 +728,7 @@
     <col min="10" max="10" width="20" customWidth="1"/>
     <col min="11" max="11" width="22.5" customWidth="1"/>
     <col min="12" max="12" width="12.5" customWidth="1"/>
-    <col min="13" max="13" width="13" customWidth="1"/>
+    <col min="13" max="13" width="13" style="18" customWidth="1"/>
     <col min="14" max="14" width="10" customWidth="1"/>
     <col min="15" max="15" width="18.33203125" customWidth="1"/>
     <col min="16" max="16" width="11.6640625" customWidth="1"/>
@@ -758,7 +772,7 @@
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="17" t="s">
         <v>12</v>
       </c>
       <c r="N1" s="2" t="s">
@@ -828,6 +842,9 @@
       <c r="K3" s="6" t="s">
         <v>26</v>
       </c>
+      <c r="N3" s="19" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
@@ -851,6 +868,9 @@
       <c r="J4" s="6" t="s">
         <v>25</v>
       </c>
+      <c r="N4" s="19" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
@@ -891,6 +911,9 @@
       <c r="E6" s="5" t="b">
         <v>0</v>
       </c>
+      <c r="M6" s="18">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
@@ -962,6 +985,9 @@
       </c>
       <c r="K9" s="6" t="s">
         <v>36</v>
+      </c>
+      <c r="N9" s="19" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add extra field to Rcvd Date
</commit_message>
<xml_diff>
--- a/mapping_spreadsheet/Casrec_Mapping_Document_Reporting.xlsx
+++ b/mapping_spreadsheet/Casrec_Mapping_Document_Reporting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifermackown/Documents/work/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{071CBA14-C2D0-034E-A020-CE60BF77528B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99B56EE0-9103-DE47-AD4D-0A065EFBC506}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="6" r:id="rId1"/>
@@ -339,54 +339,55 @@
     <t>annualreport_id</t>
   </si>
   <si>
-    <t>Rcvd Date1
+    <t>get_max_col</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>current_date</t>
+  </si>
+  <si>
+    <t>mapping_file_name</t>
+  </si>
+  <si>
+    <t>entity_name</t>
+  </si>
+  <si>
+    <t>required_entities</t>
+  </si>
+  <si>
+    <t>destination_table_name</t>
+  </si>
+  <si>
+    <t>table_type</t>
+  </si>
+  <si>
+    <t>source_table_name</t>
+  </si>
+  <si>
+    <t>casrec_conditions</t>
+  </si>
+  <si>
+    <t>source_table_additional_columns</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>Case</t>
+  </si>
+  <si>
+    <t>account</t>
+  </si>
+  <si>
+    <t>Rcvd Date
+Rcvd Date1
 Rcvd Date2
 Rcvd Date3
 Rcvd Date4
 Rcvd Date5
 Rcvd Date6</t>
-  </si>
-  <si>
-    <t>get_max_col</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>current_date</t>
-  </si>
-  <si>
-    <t>mapping_file_name</t>
-  </si>
-  <si>
-    <t>entity_name</t>
-  </si>
-  <si>
-    <t>required_entities</t>
-  </si>
-  <si>
-    <t>destination_table_name</t>
-  </si>
-  <si>
-    <t>table_type</t>
-  </si>
-  <si>
-    <t>source_table_name</t>
-  </si>
-  <si>
-    <t>casrec_conditions</t>
-  </si>
-  <si>
-    <t>source_table_additional_columns</t>
-  </si>
-  <si>
-    <t>data</t>
-  </si>
-  <si>
-    <t>Case</t>
-  </si>
-  <si>
-    <t>account</t>
   </si>
 </sst>
 </file>
@@ -758,7 +759,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE371035-1C42-914F-8247-28923EC5B10E}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
@@ -766,28 +767,28 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="C1" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="D1" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="E1" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="F1" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="G1" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="H1" s="20" t="s">
         <v>114</v>
-      </c>
-      <c r="H1" s="20" t="s">
-        <v>115</v>
       </c>
       <c r="I1" s="21"/>
     </row>
@@ -802,13 +803,13 @@
         <v>17</v>
       </c>
       <c r="E2" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="H2" s="22" t="s">
         <v>116</v>
-      </c>
-      <c r="F2" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="H2" s="22" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
@@ -822,10 +823,10 @@
         <v>61</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F3" s="22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -838,9 +839,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M1" sqref="M1:M1048576"/>
+      <selection pane="bottomLeft" activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -972,7 +973,7 @@
         <v>26</v>
       </c>
       <c r="N3" s="19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -998,7 +999,7 @@
         <v>25</v>
       </c>
       <c r="N4" s="19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1116,7 +1117,7 @@
         <v>36</v>
       </c>
       <c r="N9" s="19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1179,13 +1180,13 @@
         <v>24</v>
       </c>
       <c r="J12" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="K12" t="s">
         <v>104</v>
       </c>
-      <c r="K12" t="s">
+      <c r="P12" t="s">
         <v>105</v>
-      </c>
-      <c r="P12" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
moved the table def into a folder - keep it out of the way of the normal defs changed a couple of fields to default to the current_date
</commit_message>
<xml_diff>
--- a/mapping_spreadsheet/Casrec_Mapping_Document_Reporting.xlsx
+++ b/mapping_spreadsheet/Casrec_Mapping_Document_Reporting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifermackown/Documents/work/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99B56EE0-9103-DE47-AD4D-0A065EFBC506}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC67716-1DE1-F74A-8138-79991A8A40D3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="116">
   <si>
     <t>table_name</t>
   </si>
@@ -105,9 +105,6 @@
     <t>End Date</t>
   </si>
   <si>
-    <t>calculate_duedate</t>
-  </si>
-  <si>
     <t>reportingperiodenddate</t>
   </si>
   <si>
@@ -129,13 +126,7 @@
     <t>reportduereminderdate</t>
   </si>
   <si>
-    <t>calculate_reminderdate</t>
-  </si>
-  <si>
     <t>reportingperiodstartdate</t>
-  </si>
-  <si>
-    <t>calculate_startdate</t>
   </si>
   <si>
     <t>client_id</t>
@@ -767,28 +758,28 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="D1" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="E1" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="F1" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="G1" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="H1" s="20" t="s">
         <v>111</v>
-      </c>
-      <c r="F1" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="H1" s="20" t="s">
-        <v>114</v>
       </c>
       <c r="I1" s="21"/>
     </row>
@@ -803,30 +794,30 @@
         <v>17</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="H2" s="22" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B3" s="22" t="s">
         <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F3" s="22" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -841,7 +832,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J12" sqref="J12"/>
+      <selection pane="bottomLeft" activeCell="P13" sqref="P13:P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -963,17 +954,13 @@
       <c r="E3" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="H3" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="H3" s="6"/>
       <c r="I3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="K3" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="K3" s="6"/>
       <c r="N3" s="19" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -984,7 +971,7 @@
         <v>18</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>23</v>
@@ -999,7 +986,7 @@
         <v>25</v>
       </c>
       <c r="N4" s="19" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1010,7 +997,7 @@
         <v>18</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>23</v>
@@ -1022,7 +1009,7 @@
         <v>24</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1033,7 +1020,7 @@
         <v>18</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>20</v>
@@ -1053,7 +1040,7 @@
         <v>18</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>20</v>
@@ -1062,7 +1049,7 @@
         <v>0</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1073,7 +1060,7 @@
         <v>18</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>23</v>
@@ -1087,9 +1074,7 @@
       <c r="I8" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="K8" s="6" t="s">
-        <v>34</v>
-      </c>
+      <c r="K8" s="6"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
@@ -1099,7 +1084,7 @@
         <v>18</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>23</v>
@@ -1113,11 +1098,9 @@
       <c r="I9" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="K9" s="6" t="s">
-        <v>36</v>
-      </c>
+      <c r="K9" s="6"/>
       <c r="N9" s="19" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1128,7 +1111,7 @@
         <v>18</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>20</v>
@@ -1137,10 +1120,10 @@
         <v>0</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1151,10 +1134,10 @@
         <v>18</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E11" s="5" t="b">
         <v>0</v>
@@ -1168,7 +1151,7 @@
         <v>18</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>23</v>
@@ -1180,13 +1163,13 @@
         <v>24</v>
       </c>
       <c r="J12" s="16" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="K12" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="P12" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1197,7 +1180,7 @@
         <v>18</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>23</v>
@@ -1214,10 +1197,10 @@
         <v>18</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E14" s="5" t="b">
         <v>0</v>
@@ -1231,10 +1214,10 @@
         <v>18</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E15" s="5" t="b">
         <v>0</v>
@@ -1248,10 +1231,10 @@
         <v>18</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E16" s="5" t="b">
         <v>0</v>
@@ -1260,16 +1243,14 @@
         <v>24</v>
       </c>
       <c r="J16" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="L16" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6" t="s">
         <v>47</v>
-      </c>
-      <c r="L16" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="P16" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q16" s="6" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1280,14 +1261,15 @@
         <v>18</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E17" s="5" t="b">
         <v>0</v>
       </c>
+      <c r="P17" s="10"/>
     </row>
     <row r="18" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
@@ -1297,14 +1279,15 @@
         <v>18</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E18" s="5" t="b">
         <v>0</v>
       </c>
+      <c r="P18" s="10"/>
     </row>
     <row r="19" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
@@ -1314,14 +1297,15 @@
         <v>18</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E19" s="5" t="b">
         <v>0</v>
       </c>
+      <c r="P19" s="10"/>
     </row>
     <row r="20" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
@@ -1331,7 +1315,7 @@
         <v>18</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>23</v>
@@ -1343,8 +1327,9 @@
         <v>24</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>55</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="P20" s="10"/>
     </row>
     <row r="21" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
@@ -1354,7 +1339,7 @@
         <v>18</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>20</v>
@@ -1363,8 +1348,9 @@
         <v>0</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>57</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="P21" s="10"/>
     </row>
     <row r="22" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
@@ -1374,7 +1360,7 @@
         <v>18</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>20</v>
@@ -1383,13 +1369,11 @@
         <v>0</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="P22" s="6" t="s">
-        <v>49</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="P22" s="10"/>
       <c r="Q22" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2866,7 +2850,7 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>18</v>
@@ -2883,13 +2867,13 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>20</v>
@@ -2898,38 +2882,38 @@
         <v>0</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E4" s="5" t="b">
         <v>0</v>
       </c>
       <c r="P4" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>23</v>
@@ -2938,47 +2922,47 @@
         <v>0</v>
       </c>
       <c r="H5" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="P5" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q5" s="6" t="s">
         <v>68</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="P5" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q5" s="6" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E6" s="5" t="b">
         <v>0</v>
       </c>
       <c r="P6" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>23</v>
@@ -2987,79 +2971,79 @@
         <v>0</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="P7" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E8" s="5" t="b">
         <v>0</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="P8" s="6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="Q8" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E9" s="5" t="b">
         <v>0</v>
       </c>
       <c r="P9" s="6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="Q9" s="6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>23</v>
@@ -3068,21 +3052,21 @@
         <v>0</v>
       </c>
       <c r="P10" s="6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="Q10" s="6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>23</v>
@@ -3091,27 +3075,27 @@
         <v>0</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="P11" s="6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="Q11" s="6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>20</v>
@@ -3120,13 +3104,13 @@
         <v>0</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="P12" s="6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="Q12" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4555,16 +4539,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4573,10 +4557,10 @@
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="14" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5603,93 +5587,93 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="10" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="10" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="10" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="10" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="10" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="10" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="10" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6783,7 +6767,7 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>18</v>
@@ -6800,16 +6784,16 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E3" s="5" t="b">
         <v>0</v>
@@ -6817,16 +6801,16 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E4" s="5" t="b">
         <v>0</v>
@@ -6834,16 +6818,16 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E5" s="5" t="b">
         <v>0</v>
@@ -6851,13 +6835,13 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>20</v>
@@ -6866,7 +6850,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Add mapping for reporting dates
</commit_message>
<xml_diff>
--- a/mapping_spreadsheet/Casrec_Mapping_Document_Reporting.xlsx
+++ b/mapping_spreadsheet/Casrec_Mapping_Document_Reporting.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifermackown/Documents/work/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliotsmith/projects/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC67716-1DE1-F74A-8138-79991A8A40D3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8703FF54-F97B-744C-AD23-EAD0F59E881C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="460" windowWidth="38400" windowHeight="19440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="6" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="121">
   <si>
     <t>table_name</t>
   </si>
@@ -334,9 +334,6 @@
   </si>
   <si>
     <t>yes</t>
-  </si>
-  <si>
-    <t>current_date</t>
   </si>
   <si>
     <t>mapping_file_name</t>
@@ -379,6 +376,24 @@
 Rcvd Date4
 Rcvd Date5
 Rcvd Date6</t>
+  </si>
+  <si>
+    <t>calculate_date:reportingperiodenddate+21|next-working-day</t>
+  </si>
+  <si>
+    <t>calculate_date:reportingperiodenddate-21|previous-working-day</t>
+  </si>
+  <si>
+    <t>calculate_date:reportingperiodenddate-366</t>
+  </si>
+  <si>
+    <t>21 days before reportingperiodenddate, or closest previous working day if that falls on a weekend</t>
+  </si>
+  <si>
+    <t>21 days after reportingperiodenddate, or closest next working day if that falls on a weekend</t>
+  </si>
+  <si>
+    <t>366 days before reportingperiodenddate</t>
   </si>
 </sst>
 </file>
@@ -758,28 +773,28 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="C1" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="D1" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="E1" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="F1" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="G1" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="H1" s="20" t="s">
         <v>110</v>
-      </c>
-      <c r="H1" s="20" t="s">
-        <v>111</v>
       </c>
       <c r="I1" s="21"/>
     </row>
@@ -794,13 +809,13 @@
         <v>17</v>
       </c>
       <c r="E2" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="H2" s="22" t="s">
         <v>112</v>
-      </c>
-      <c r="F2" s="22" t="s">
-        <v>114</v>
-      </c>
-      <c r="H2" s="22" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
@@ -814,10 +829,10 @@
         <v>58</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F3" s="22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -832,7 +847,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P13" sqref="P13:P22"/>
+      <selection pane="bottomLeft" activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -850,7 +865,7 @@
     <col min="11" max="11" width="22.5" customWidth="1"/>
     <col min="12" max="12" width="12.5" customWidth="1"/>
     <col min="13" max="13" width="13" style="18" customWidth="1"/>
-    <col min="14" max="14" width="10" customWidth="1"/>
+    <col min="14" max="14" width="54.33203125" customWidth="1"/>
     <col min="15" max="15" width="18.33203125" customWidth="1"/>
     <col min="16" max="16" width="11.6640625" customWidth="1"/>
     <col min="17" max="17" width="10.33203125" customWidth="1"/>
@@ -959,8 +974,11 @@
         <v>25</v>
       </c>
       <c r="K3" s="6"/>
-      <c r="N3" s="19" t="s">
-        <v>103</v>
+      <c r="N3" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q3" s="22" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -985,9 +1003,7 @@
       <c r="J4" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="N4" s="19" t="s">
-        <v>103</v>
-      </c>
+      <c r="N4" s="19"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
@@ -1075,6 +1091,12 @@
         <v>25</v>
       </c>
       <c r="K8" s="6"/>
+      <c r="N8" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q8" s="22" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
@@ -1099,8 +1121,11 @@
         <v>25</v>
       </c>
       <c r="K9" s="6"/>
-      <c r="N9" s="19" t="s">
-        <v>103</v>
+      <c r="N9" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q9" s="22" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1163,7 +1188,7 @@
         <v>24</v>
       </c>
       <c r="J12" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K12" t="s">
         <v>101</v>

</xml_diff>

<commit_message>
Use transform instead of calculation
Rather than use a new type of calculation to derive dates for
reporting, use new transforms.
</commit_message>
<xml_diff>
--- a/mapping_spreadsheet/Casrec_Mapping_Document_Reporting.xlsx
+++ b/mapping_spreadsheet/Casrec_Mapping_Document_Reporting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliotsmith/projects/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8703FF54-F97B-744C-AD23-EAD0F59E881C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC1D883E-C128-8E4A-8772-F27FF914A62B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="460" windowWidth="38400" windowHeight="19440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="121">
   <si>
     <t>table_name</t>
   </si>
@@ -378,15 +378,6 @@
 Rcvd Date6</t>
   </si>
   <si>
-    <t>calculate_date:reportingperiodenddate+21|next-working-day</t>
-  </si>
-  <si>
-    <t>calculate_date:reportingperiodenddate-21|previous-working-day</t>
-  </si>
-  <si>
-    <t>calculate_date:reportingperiodenddate-366</t>
-  </si>
-  <si>
     <t>21 days before reportingperiodenddate, or closest previous working day if that falls on a weekend</t>
   </si>
   <si>
@@ -394,6 +385,15 @@
   </si>
   <si>
     <t>366 days before reportingperiodenddate</t>
+  </si>
+  <si>
+    <t>calculate_startdate</t>
+  </si>
+  <si>
+    <t>calculate_reminderdate</t>
+  </si>
+  <si>
+    <t>calculate_duedate</t>
   </si>
 </sst>
 </file>
@@ -770,6 +770,10 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="4" max="4" width="25.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="20" t="s">
@@ -847,7 +851,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q9" sqref="Q9"/>
+      <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -865,7 +869,7 @@
     <col min="11" max="11" width="22.5" customWidth="1"/>
     <col min="12" max="12" width="12.5" customWidth="1"/>
     <col min="13" max="13" width="13" style="18" customWidth="1"/>
-    <col min="14" max="14" width="54.33203125" customWidth="1"/>
+    <col min="14" max="14" width="23.33203125" customWidth="1"/>
     <col min="15" max="15" width="18.33203125" customWidth="1"/>
     <col min="16" max="16" width="11.6640625" customWidth="1"/>
     <col min="17" max="17" width="10.33203125" customWidth="1"/>
@@ -969,16 +973,24 @@
       <c r="E3" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="H3" s="6"/>
+      <c r="H3" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="I3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="K3" s="6"/>
-      <c r="N3" s="22" t="s">
-        <v>115</v>
+      <c r="J3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="N3" s="22"/>
+      <c r="P3" t="s">
+        <v>102</v>
       </c>
       <c r="Q3" s="22" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1004,6 +1016,9 @@
         <v>25</v>
       </c>
       <c r="N4" s="19"/>
+      <c r="P4" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
@@ -1090,12 +1105,18 @@
       <c r="I8" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="K8" s="6"/>
-      <c r="N8" s="22" t="s">
-        <v>116</v>
+      <c r="J8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="N8" s="22"/>
+      <c r="P8" t="s">
+        <v>102</v>
       </c>
       <c r="Q8" s="22" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1120,12 +1141,18 @@
       <c r="I9" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="K9" s="6"/>
-      <c r="N9" s="22" t="s">
+      <c r="J9" t="s">
+        <v>25</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="N9" s="22"/>
+      <c r="P9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q9" s="22" t="s">
         <v>117</v>
-      </c>
-      <c r="Q9" s="22" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Mark all fields known complete
</commit_message>
<xml_diff>
--- a/mapping_spreadsheet/Casrec_Mapping_Document_Reporting.xlsx
+++ b/mapping_spreadsheet/Casrec_Mapping_Document_Reporting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliotsmith/projects/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC1D883E-C128-8E4A-8772-F27FF914A62B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C2FEDA2-73A4-C44F-BD50-4D298149480F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="460" windowWidth="38400" windowHeight="19440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="121">
   <si>
     <t>table_name</t>
   </si>
@@ -851,7 +851,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
+      <selection pane="bottomLeft" activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1381,7 +1381,9 @@
       <c r="J20" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="P20" s="10"/>
+      <c r="P20" s="10" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="21" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">

</xml_diff>

<commit_message>
Update revstatus_lookup to use PHP constants
</commit_message>
<xml_diff>
--- a/mapping_spreadsheet/Casrec_Mapping_Document_Reporting.xlsx
+++ b/mapping_spreadsheet/Casrec_Mapping_Document_Reporting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliotsmith/projects/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6867B81B-97EA-FA40-8A48-4E16E1A35F55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F54B6B-1D38-7E4C-8DA2-1CE93B7F90EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="460" windowWidth="38400" windowHeight="19440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="460" windowWidth="38400" windowHeight="19440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="6" r:id="rId1"/>
@@ -390,20 +390,20 @@
     <t>no</t>
   </si>
   <si>
-    <t>Staff: referred</t>
-  </si>
-  <si>
-    <t>No Review</t>
-  </si>
-  <si>
-    <t>Reviewed</t>
+    <t>STAFF_REFERRED</t>
+  </si>
+  <si>
+    <t>NO_REVIEW</t>
+  </si>
+  <si>
+    <t>REVIEWED</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -469,6 +469,11 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Menlo"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -539,7 +544,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -609,6 +614,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -910,7 +916,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="R6" sqref="R6"/>
     </sheetView>
@@ -5697,13 +5703,15 @@
   </sheetPr>
   <dimension ref="A1:D990"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="6" width="14.5" customWidth="1"/>
+    <col min="1" max="3" width="14.5" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
+    <col min="5" max="6" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5720,7 +5728,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
         <v>86</v>
       </c>
@@ -5730,11 +5738,11 @@
       <c r="C2" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="35" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
         <v>88</v>
       </c>
@@ -5744,11 +5752,11 @@
       <c r="C3" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="35" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
         <v>89</v>
       </c>
@@ -5758,7 +5766,7 @@
       <c r="C4" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="35" t="s">
         <v>121</v>
       </c>
     </row>

</xml_diff>